<commit_message>
[Create]migration Tables to mysql DB
</commit_message>
<xml_diff>
--- a/doc/TableDesign/TableDesign.xlsx
+++ b/doc/TableDesign/TableDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Soft\WebAppSample\doc\TableDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C449D188-3CDE-4739-9A63-FCF4212CF286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C693E0A9-2FCD-4042-896F-6A02EA40BFEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{F698256D-8130-4C08-A905-749CD078375B}"/>
+    <workbookView xWindow="4680" yWindow="14290" windowWidth="19420" windowHeight="10300" xr2:uid="{F698256D-8130-4C08-A905-749CD078375B}"/>
   </bookViews>
   <sheets>
     <sheet name="データ作成&amp;取得の検証" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -942,7 +940,7 @@
   <dimension ref="A1:L71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O49" sqref="O49"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>